<commit_message>
finishing barcodeprint (front for now)
</commit_message>
<xml_diff>
--- a/Autostockin (break - urgent)/ยิงรับ 49.xlsx
+++ b/Autostockin (break - urgent)/ยิงรับ 49.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workstuff\my-work-python-script\Autostockin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workstuff\my-work-python-script\Autostockin (break - urgent)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDDC6E8-B956-40A0-ADB9-9FC0D3292725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30501EAF-EFD2-43E9-B224-F7E38A35A254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{47EFCF22-5A4D-4004-9D3D-F4E18B203E38}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5156" uniqueCount="3754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5194" uniqueCount="3792">
   <si>
     <t xml:space="preserve">Bill Type: </t>
   </si>
@@ -11300,6 +11300,120 @@
   </si>
   <si>
     <t>+1311-1072</t>
+  </si>
+  <si>
+    <t>+985-578</t>
+  </si>
+  <si>
+    <t>+16167-212</t>
+  </si>
+  <si>
+    <t>+665-1245</t>
+  </si>
+  <si>
+    <t>+15877-80</t>
+  </si>
+  <si>
+    <t>+3988-699</t>
+  </si>
+  <si>
+    <t>+14849-335</t>
+  </si>
+  <si>
+    <t>+4965-663</t>
+  </si>
+  <si>
+    <t>+611-2070</t>
+  </si>
+  <si>
+    <t>+1616-1376</t>
+  </si>
+  <si>
+    <t>+24413-365</t>
+  </si>
+  <si>
+    <t>+2902-1211</t>
+  </si>
+  <si>
+    <t>+2975-672</t>
+  </si>
+  <si>
+    <t>+1173-1237</t>
+  </si>
+  <si>
+    <t>+666-1245</t>
+  </si>
+  <si>
+    <t>+555-1329</t>
+  </si>
+  <si>
+    <t>+1304-2065</t>
+  </si>
+  <si>
+    <t>4598-1205</t>
+  </si>
+  <si>
+    <t>+21778-182</t>
+  </si>
+  <si>
+    <t>+816-1167</t>
+  </si>
+  <si>
+    <t>+12368-314</t>
+  </si>
+  <si>
+    <t>+6382-664</t>
+  </si>
+  <si>
+    <t>+150-1502</t>
+  </si>
+  <si>
+    <t>+1660-574</t>
+  </si>
+  <si>
+    <t>+5638-469</t>
+  </si>
+  <si>
+    <t>+3616-975</t>
+  </si>
+  <si>
+    <t>+1354-1308</t>
+  </si>
+  <si>
+    <t>+651-1271</t>
+  </si>
+  <si>
+    <t>+3770-488</t>
+  </si>
+  <si>
+    <t>+13209-477</t>
+  </si>
+  <si>
+    <t>+1089-1081</t>
+  </si>
+  <si>
+    <t>+1463-886</t>
+  </si>
+  <si>
+    <t>+19486-459</t>
+  </si>
+  <si>
+    <t>+1168-591</t>
+  </si>
+  <si>
+    <t>+22955-207</t>
+  </si>
+  <si>
+    <t>+6722-370</t>
+  </si>
+  <si>
+    <t>+0097-1535</t>
+  </si>
+  <si>
+    <t>+12707-191</t>
+  </si>
+  <si>
+    <t>+8394-635</t>
   </si>
 </sst>
 </file>
@@ -11678,10 +11792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B40E757-AF6D-418F-8CB6-C916F96CFF4A}">
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12181,67 +12295,215 @@
       <c r="G88" s="1"/>
     </row>
     <row r="89" spans="1:7">
+      <c r="A89" s="1" t="s">
+        <v>3754</v>
+      </c>
       <c r="G89" s="1"/>
     </row>
     <row r="90" spans="1:7">
+      <c r="A90" s="1" t="s">
+        <v>3755</v>
+      </c>
       <c r="G90" s="1"/>
     </row>
     <row r="91" spans="1:7">
+      <c r="A91" s="1" t="s">
+        <v>3756</v>
+      </c>
       <c r="G91" s="1"/>
     </row>
     <row r="92" spans="1:7">
+      <c r="A92" s="1" t="s">
+        <v>3757</v>
+      </c>
       <c r="G92" s="1"/>
     </row>
     <row r="93" spans="1:7">
+      <c r="A93" s="1" t="s">
+        <v>3758</v>
+      </c>
       <c r="G93" s="1"/>
     </row>
     <row r="94" spans="1:7">
+      <c r="A94" s="1" t="s">
+        <v>3759</v>
+      </c>
       <c r="G94" s="1"/>
     </row>
     <row r="95" spans="1:7">
+      <c r="A95" s="1" t="s">
+        <v>3760</v>
+      </c>
       <c r="G95" s="1"/>
     </row>
     <row r="96" spans="1:7">
+      <c r="A96" s="1" t="s">
+        <v>3761</v>
+      </c>
       <c r="G96" s="1"/>
     </row>
-    <row r="97" spans="7:7">
+    <row r="97" spans="1:7">
+      <c r="A97" s="1" t="s">
+        <v>3762</v>
+      </c>
       <c r="G97" s="1"/>
     </row>
-    <row r="98" spans="7:7">
+    <row r="98" spans="1:7">
+      <c r="A98" s="1" t="s">
+        <v>3763</v>
+      </c>
       <c r="G98" s="1"/>
     </row>
-    <row r="99" spans="7:7">
+    <row r="99" spans="1:7">
+      <c r="A99" s="1" t="s">
+        <v>3764</v>
+      </c>
       <c r="G99" s="1"/>
     </row>
-    <row r="100" spans="7:7">
+    <row r="100" spans="1:7">
+      <c r="A100" s="1" t="s">
+        <v>3765</v>
+      </c>
       <c r="G100" s="1"/>
     </row>
-    <row r="101" spans="7:7">
+    <row r="101" spans="1:7">
+      <c r="A101" s="1" t="s">
+        <v>3766</v>
+      </c>
       <c r="G101" s="1"/>
     </row>
-    <row r="102" spans="7:7">
+    <row r="102" spans="1:7">
+      <c r="A102" s="1" t="s">
+        <v>3767</v>
+      </c>
       <c r="G102" s="1"/>
     </row>
-    <row r="103" spans="7:7">
+    <row r="103" spans="1:7">
+      <c r="A103" s="1" t="s">
+        <v>3768</v>
+      </c>
       <c r="G103" s="1"/>
     </row>
-    <row r="104" spans="7:7">
+    <row r="104" spans="1:7">
+      <c r="A104" s="1" t="s">
+        <v>3769</v>
+      </c>
       <c r="G104" s="1"/>
     </row>
-    <row r="105" spans="7:7">
+    <row r="105" spans="1:7">
+      <c r="A105" s="1" t="s">
+        <v>3770</v>
+      </c>
       <c r="G105" s="1"/>
     </row>
-    <row r="106" spans="7:7">
+    <row r="106" spans="1:7">
+      <c r="A106" s="1" t="s">
+        <v>3771</v>
+      </c>
       <c r="G106" s="1"/>
     </row>
-    <row r="107" spans="7:7">
+    <row r="107" spans="1:7">
+      <c r="A107" s="1" t="s">
+        <v>3772</v>
+      </c>
       <c r="G107" s="1"/>
     </row>
-    <row r="108" spans="7:7">
+    <row r="108" spans="1:7">
+      <c r="A108" s="1" t="s">
+        <v>3773</v>
+      </c>
       <c r="G108" s="1"/>
     </row>
-    <row r="109" spans="7:7">
+    <row r="109" spans="1:7">
+      <c r="A109" s="1" t="s">
+        <v>3774</v>
+      </c>
       <c r="G109" s="1"/>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" s="1" t="s">
+        <v>3775</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" s="1" t="s">
+        <v>3776</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" s="1" t="s">
+        <v>3777</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="1" t="s">
+        <v>3778</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="1" t="s">
+        <v>3779</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="1" t="s">
+        <v>3780</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="1" t="s">
+        <v>3781</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="1" t="s">
+        <v>3782</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="1" t="s">
+        <v>3783</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="1" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="1" t="s">
+        <v>3785</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="1" t="s">
+        <v>3786</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="1" t="s">
+        <v>3787</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="1" t="s">
+        <v>3788</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="1" t="s">
+        <v>3789</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="1" t="s">
+        <v>3790</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="1" t="s">
+        <v>3791</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="C1:E250" xr:uid="{1B40E757-AF6D-418F-8CB6-C916F96CFF4A}"/>
@@ -22772,9 +23034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C21679-A84C-4371-A1C5-AF880A10BEAA}">
   <dimension ref="A1:U491"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8:U28"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>